<commit_message>
Main sequence -> Main flowchart
</commit_message>
<xml_diff>
--- a/NewEmployeeBestMatch/Data/Config.xlsx
+++ b/NewEmployeeBestMatch/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CTI31x\CTI316RPA\Proiect\New-Employee-Best-Match\NewEmployeeBestMatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97128F-6497-4576-84B9-FCBF0BB13132}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6AA350-A678-4B62-BA9D-BF667D7A32D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>OrchestatorAssetFolder</t>
+  </si>
+  <si>
+    <t>downloadPath</t>
+  </si>
+  <si>
+    <t>Data\Downloads</t>
   </si>
 </sst>
 </file>
@@ -368,14 +374,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -388,6 +396,14 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -429,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6760C607-9B84-460F-A35A-3A4409A2D615}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
verify existing folder sequence
</commit_message>
<xml_diff>
--- a/NewEmployeeBestMatch/Data/Config.xlsx
+++ b/NewEmployeeBestMatch/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CTI31x\CTI316RPA\Proiect\New-Employee-Best-Match\NewEmployeeBestMatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6AA350-A678-4B62-BA9D-BF667D7A32D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0442A4-FD9B-42F3-AB01-C5695F5CAF42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Data\Downloads</t>
+  </si>
+  <si>
+    <t>LogMessage_NewFolder</t>
+  </si>
+  <si>
+    <t>The folder does not exist. It was created automatically by the system.</t>
   </si>
 </sst>
 </file>
@@ -376,7 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
@@ -414,14 +420,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6341839-9AAE-46E0-8454-A0FC0B7AC587}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -434,6 +442,14 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verify existing folder update
</commit_message>
<xml_diff>
--- a/NewEmployeeBestMatch/Data/Config.xlsx
+++ b/NewEmployeeBestMatch/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CTI31x\CTI316RPA\Proiect\New-Employee-Best-Match\NewEmployeeBestMatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0442A4-FD9B-42F3-AB01-C5695F5CAF42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C6ED8F-522F-4E7E-B74A-66640FFF7EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -50,17 +50,77 @@
     <t>Data\Downloads</t>
   </si>
   <si>
-    <t>LogMessage_NewFolder</t>
-  </si>
-  <si>
     <t>The folder does not exist. It was created automatically by the system.</t>
+  </si>
+  <si>
+    <t>cvDownloadPath</t>
+  </si>
+  <si>
+    <t>jobDownloadPath</t>
+  </si>
+  <si>
+    <t>Data\Downloads\Jobs</t>
+  </si>
+  <si>
+    <t>Data\Downloads\CVs</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>rpa_project@outlook.com</t>
+  </si>
+  <si>
+    <t>emailFolder</t>
+  </si>
+  <si>
+    <t>Inbox</t>
+  </si>
+  <si>
+    <t>logMessageNewFolder</t>
+  </si>
+  <si>
+    <t>logMessageNewFile</t>
+  </si>
+  <si>
+    <t>The file does not exist. It was created automatically by the system.</t>
+  </si>
+  <si>
+    <t>logMessageReadEmails</t>
+  </si>
+  <si>
+    <t>Reading the emails…</t>
+  </si>
+  <si>
+    <t>logMessageVerifyExistingFolder</t>
+  </si>
+  <si>
+    <t>Verifying existence of folder…</t>
+  </si>
+  <si>
+    <t>logMessageInitAllSettings</t>
+  </si>
+  <si>
+    <t>Initializing all settings…</t>
+  </si>
+  <si>
+    <t>replyMessageNoAttachment</t>
+  </si>
+  <si>
+    <t>replyMessageConfirmation</t>
+  </si>
+  <si>
+    <t>We have received the email sent by you.</t>
+  </si>
+  <si>
+    <t>The mail you sent does not include an attachment.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +132,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,14 +162,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -380,16 +451,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -406,29 +477,40 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{8BEBC1BA-E4E0-4227-8AE8-1D6A22B9E73E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6341839-9AAE-46E0-8454-A0FC0B7AC587}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -446,10 +528,82 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Document Understanding - Added
</commit_message>
<xml_diff>
--- a/NewEmployeeBestMatch/Data/Config.xlsx
+++ b/NewEmployeeBestMatch/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CTI31x\CTI316RPA\Proiect\New-Employee-Best-Match\NewEmployeeBestMatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C6ED8F-522F-4E7E-B74A-66640FFF7EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08C5357-AC14-4DC0-AA6E-D93F7DF1EC88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3192" yWindow="1452" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>The mail you sent does not include an attachment.</t>
+  </si>
+  <si>
+    <t>keywordDocumentPath</t>
+  </si>
+  <si>
+    <t>DocumentProcessing\keyword.json</t>
   </si>
 </sst>
 </file>
@@ -502,10 +508,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6341839-9AAE-46E0-8454-A0FC0B7AC587}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,19 +596,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DataTables generation based on DocumentUnderstanding OCR
</commit_message>
<xml_diff>
--- a/NewEmployeeBestMatch/Data/Config.xlsx
+++ b/NewEmployeeBestMatch/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CTI31x\CTI316RPA\Proiect\New-Employee-Best-Match\NewEmployeeBestMatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B23D439-2CF6-4EA0-9734-E755E44F44CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3B26F7-163B-40DE-AEB7-3363F7C2CDFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3192" yWindow="1452" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -126,6 +126,30 @@
   </si>
   <si>
     <t>aZJUCNiGx5TWK04asE1ExtUD7qm2iGnoIK/TcPP1SQmg+H6xF2aklCmLDl1HPyL17qpVEsN0EeLW8/OsWs64fQ==</t>
+  </si>
+  <si>
+    <t>jobIndexPath</t>
+  </si>
+  <si>
+    <t>cvIndexPath</t>
+  </si>
+  <si>
+    <t>jobFolderPath</t>
+  </si>
+  <si>
+    <t>cvFolderPath</t>
+  </si>
+  <si>
+    <t>Data\Index\Jobs</t>
+  </si>
+  <si>
+    <t>Data\Index\CVs</t>
+  </si>
+  <si>
+    <t>Data\Index\Jobs\jobs.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Index\CVs\CVs.xlsx</t>
   </si>
 </sst>
 </file>
@@ -514,16 +538,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6341839-9AAE-46E0-8454-A0FC0B7AC587}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -610,27 +634,59 @@
         <v>30</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generate List of Future Employees and Send to the Company
</commit_message>
<xml_diff>
--- a/NewEmployeeBestMatch/Data/Config.xlsx
+++ b/NewEmployeeBestMatch/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CTI31x\CTI316RPA\Proiect\New-Employee-Best-Match\NewEmployeeBestMatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3B26F7-163B-40DE-AEB7-3363F7C2CDFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9C14E4-1EE4-4B84-B263-3D69B9FE338E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,28 +128,28 @@
     <t>aZJUCNiGx5TWK04asE1ExtUD7qm2iGnoIK/TcPP1SQmg+H6xF2aklCmLDl1HPyL17qpVEsN0EeLW8/OsWs64fQ==</t>
   </si>
   <si>
-    <t>jobIndexPath</t>
-  </si>
-  <si>
-    <t>cvIndexPath</t>
-  </si>
-  <si>
     <t>jobFolderPath</t>
   </si>
   <si>
     <t>cvFolderPath</t>
   </si>
   <si>
-    <t>Data\Index\Jobs</t>
-  </si>
-  <si>
-    <t>Data\Index\CVs</t>
-  </si>
-  <si>
-    <t>Data\Index\Jobs\jobs.xlsx</t>
-  </si>
-  <si>
-    <t>Data\Index\CVs\CVs.xlsx</t>
+    <t>Data\Archive\Jobs</t>
+  </si>
+  <si>
+    <t>Data\Archive\CVs</t>
+  </si>
+  <si>
+    <t>Data\Employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi! This is the list of potential future employees for the job with the id: </t>
+  </si>
+  <si>
+    <t>employeesListsPath</t>
+  </si>
+  <si>
+    <t>emailMessageEmployeesList</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,50 +636,50 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Log messages - 95% complete project
</commit_message>
<xml_diff>
--- a/NewEmployeeBestMatch/Data/Config.xlsx
+++ b/NewEmployeeBestMatch/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CTI31x\CTI316RPA\Proiect\New-Employee-Best-Match\NewEmployeeBestMatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9C14E4-1EE4-4B84-B263-3D69B9FE338E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CD936C-2375-49E6-8EA7-4E1371BEED61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -150,6 +150,42 @@
   </si>
   <si>
     <t>emailMessageEmployeesList</t>
+  </si>
+  <si>
+    <t>logMessageExtractDataJob</t>
+  </si>
+  <si>
+    <t>Starting the data extraction of jobs download folder…</t>
+  </si>
+  <si>
+    <t>logMessageExtractDataCV</t>
+  </si>
+  <si>
+    <t>Starting the data extraction of CVs download folder…</t>
+  </si>
+  <si>
+    <t>logMessageDocumentUnderstanding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starting Document Understanding: </t>
+  </si>
+  <si>
+    <t>logMessageMoveFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moving the file to the archive: </t>
+  </si>
+  <si>
+    <t>logGenerateExcelFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generating the Excel File: </t>
+  </si>
+  <si>
+    <t>logSendingEmail</t>
+  </si>
+  <si>
+    <t>Sending the email…</t>
   </si>
 </sst>
 </file>
@@ -538,15 +574,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6341839-9AAE-46E0-8454-A0FC0B7AC587}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="96.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -604,89 +640,137 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B32" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Status: 100% | try-catch blocks added
</commit_message>
<xml_diff>
--- a/NewEmployeeBestMatch/Data/Config.xlsx
+++ b/NewEmployeeBestMatch/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CTI31x\CTI316RPA\Proiect\New-Employee-Best-Match\NewEmployeeBestMatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CD936C-2375-49E6-8EA7-4E1371BEED61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEFF40B-AC7F-463F-99A8-BDEE765FD18A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,12 +577,12 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="96.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>